<commit_message>
version A1 - preproduction beta
</commit_message>
<xml_diff>
--- a/Production.xlsx
+++ b/Production.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TIMELINE" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="303">
   <si>
     <t>REFERENCE DESCRIPTOR</t>
   </si>
@@ -32,27 +32,15 @@
     <t>PATTERN TYPE</t>
   </si>
   <si>
-    <t>VENDOR A</t>
-  </si>
-  <si>
     <t>MFG #</t>
   </si>
   <si>
-    <t>VEND A #</t>
-  </si>
-  <si>
     <t>$1K</t>
   </si>
   <si>
     <t>$10K</t>
   </si>
   <si>
-    <t>VENDOR B</t>
-  </si>
-  <si>
-    <t>VEND B #</t>
-  </si>
-  <si>
     <t>$100K</t>
   </si>
   <si>
@@ -930,6 +918,15 @@
   </si>
   <si>
     <t>FULL PRODUCTION COST (2000 units)</t>
+  </si>
+  <si>
+    <t>VENDOR</t>
+  </si>
+  <si>
+    <t>VEND #</t>
+  </si>
+  <si>
+    <t>REEL QTY</t>
   </si>
 </sst>
 </file>
@@ -1443,11 +1440,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="7" topLeftCell="H8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H17:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,13 +1467,13 @@
       <c r="F1" s="40"/>
       <c r="G1" s="31"/>
       <c r="H1" s="28" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="J1" s="54" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="K1" s="54"/>
     </row>
@@ -1487,7 +1484,7 @@
       <c r="F2" s="40"/>
       <c r="G2" s="31"/>
       <c r="H2" s="28" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="I2" s="32"/>
       <c r="J2" s="33">
@@ -1504,7 +1501,7 @@
       <c r="F3" s="40"/>
       <c r="G3" s="31"/>
       <c r="H3" s="28" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="I3" s="34"/>
       <c r="J3" s="33">
@@ -1521,7 +1518,7 @@
       <c r="F4" s="40"/>
       <c r="G4" s="31"/>
       <c r="H4" s="28" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I4" s="35"/>
       <c r="J4" s="33">
@@ -1545,37 +1542,37 @@
       <c r="F6" s="40"/>
       <c r="G6" s="31"/>
       <c r="H6" s="54" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="I6" s="54"/>
       <c r="J6" s="54"/>
       <c r="K6" s="54"/>
       <c r="L6" s="54" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="M6" s="54"/>
       <c r="N6" s="54"/>
       <c r="O6" s="54"/>
       <c r="P6" s="54" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="Q6" s="54"/>
       <c r="R6" s="54"/>
       <c r="S6" s="54"/>
       <c r="T6" s="54" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="U6" s="54"/>
       <c r="V6" s="54"/>
       <c r="W6" s="54"/>
       <c r="X6" s="54" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="Y6" s="54"/>
       <c r="Z6" s="54"/>
       <c r="AA6" s="54"/>
       <c r="AB6" s="54" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AC6" s="54"/>
       <c r="AD6" s="54"/>
@@ -1583,25 +1580,25 @@
     </row>
     <row r="7" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="H7" s="28">
         <v>1</v>
@@ -1678,7 +1675,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B8" s="1">
         <f>SUM(H8:AE8)</f>
@@ -1690,7 +1687,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" ref="B9:B29" si="0">SUM(H9:AE9)</f>
@@ -1702,7 +1699,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
@@ -1734,7 +1731,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="50" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
@@ -1763,7 +1760,7 @@
     </row>
     <row r="12" spans="1:31" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B12" s="51">
         <f>SUM(B8:B11)</f>
@@ -1786,7 +1783,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
@@ -1810,7 +1807,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="47" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
@@ -1837,7 +1834,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
@@ -1858,7 +1855,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
@@ -1879,7 +1876,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="47" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
@@ -1909,7 +1906,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="47" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
@@ -1935,7 +1932,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="47" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" si="0"/>
@@ -1967,7 +1964,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="47" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B20" s="1">
         <f t="shared" si="0"/>
@@ -2000,7 +1997,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="47" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B21" s="1">
         <f t="shared" si="0"/>
@@ -2012,14 +2009,14 @@
       </c>
       <c r="E21" s="44">
         <f>BOM!C2-E17</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F21" s="45">
         <v>2000</v>
       </c>
       <c r="G21" s="44">
         <f>F21*E21</f>
-        <v>26000</v>
+        <v>30000</v>
       </c>
       <c r="Q21" s="38">
         <v>14</v>
@@ -2036,11 +2033,11 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="47" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B22" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D22" s="44">
         <f>'FEE &amp; COST SCHEDULE'!C6</f>
@@ -2057,22 +2054,22 @@
         <v>4000</v>
       </c>
       <c r="Q22" s="38">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="R22" s="38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S22" s="38">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="47" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B23" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D23" s="44">
         <f>'FEE &amp; COST SCHEDULE'!C7</f>
@@ -2089,22 +2086,22 @@
         <v>4000</v>
       </c>
       <c r="Q23" s="38">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R23" s="38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S23" s="38">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="47" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B24" s="1">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="T24" s="38">
         <v>5</v>
@@ -2113,7 +2110,7 @@
         <v>5</v>
       </c>
       <c r="V24" s="38">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W24" s="38">
         <v>0</v>
@@ -2124,7 +2121,7 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="47" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B25" s="1">
         <f t="shared" si="0"/>
@@ -2151,15 +2148,15 @@
     </row>
     <row r="26" spans="1:31" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="51" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B26" s="51">
         <f>SUM(B13:B25)</f>
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="C26" s="52">
         <f>B26*'FEE &amp; COST SCHEDULE'!C10</f>
-        <v>14400</v>
+        <v>12450</v>
       </c>
       <c r="D26" s="52">
         <f t="shared" ref="D26:G26" si="3">SUM(D13:D25)</f>
@@ -2168,12 +2165,12 @@
       <c r="E26" s="52"/>
       <c r="G26" s="52">
         <f t="shared" si="3"/>
-        <v>119078.00000000001</v>
+        <v>123078.00000000001</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B27" s="1">
         <f t="shared" si="0"/>
@@ -2200,7 +2197,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B28" s="1">
         <f t="shared" si="0"/>
@@ -2224,7 +2221,7 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B29" s="1">
         <f t="shared" si="0"/>
@@ -2245,7 +2242,7 @@
     </row>
     <row r="30" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B30" s="51">
         <f>SUM(B27:B29)</f>
@@ -2276,15 +2273,15 @@
     </row>
     <row r="32" spans="1:31" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B32" s="51">
         <f>B12+B26+B30</f>
-        <v>213</v>
+        <v>187</v>
       </c>
       <c r="C32" s="52">
         <f>C12+C26+C30</f>
-        <v>15975</v>
+        <v>14025</v>
       </c>
       <c r="D32" s="52">
         <f>D26+D12+D30</f>
@@ -2294,7 +2291,7 @@
       <c r="F32" s="51"/>
       <c r="G32" s="52">
         <f>G26+G12+G30</f>
-        <v>127478.00000000001</v>
+        <v>131478</v>
       </c>
       <c r="H32" s="51">
         <f t="shared" ref="H32:AE32" si="5">SUM(H8:H29)</f>
@@ -2334,15 +2331,15 @@
       </c>
       <c r="Q32" s="51">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="R32" s="51">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="S32" s="51">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="T32" s="51">
         <f t="shared" si="5"/>
@@ -2354,7 +2351,7 @@
       </c>
       <c r="V32" s="51">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W32" s="51">
         <f t="shared" si="5"/>
@@ -2395,11 +2392,11 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C34" s="31">
         <f>C32+D32+G32</f>
-        <v>157753</v>
+        <v>159803</v>
       </c>
     </row>
   </sheetData>
@@ -2433,7 +2430,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B1" s="53">
         <f>TIMELINE!C12+TIMELINE!D12+TIMELINE!G12</f>
@@ -2442,106 +2439,106 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B11" s="53">
         <f>TIMELINE!C26+TIMELINE!D26+TIMELINE!G26</f>
-        <v>146478</v>
+        <v>148528</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -2566,12 +2563,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C2" s="18">
         <v>500</v>
@@ -2579,7 +2576,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C3" s="18">
         <v>6000</v>
@@ -2587,7 +2584,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C4" s="18">
         <v>300</v>
@@ -2595,7 +2592,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C5" s="18">
         <v>300</v>
@@ -2603,7 +2600,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C6" s="18">
         <v>200</v>
@@ -2611,7 +2608,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C7" s="18">
         <v>200</v>
@@ -2619,12 +2616,12 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C10" s="18">
         <v>75</v>
@@ -2639,9 +2636,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2656,28 +2653,28 @@
   <sheetData>
     <row r="1" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C1" s="55" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D1" s="55"/>
       <c r="E1" s="55" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F1" s="55"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="20">
         <f>SUM(D3:D5)</f>
-        <v>48.464000000000006</v>
+        <v>50.464000000000006</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="14">
@@ -2688,11 +2685,11 @@
     </row>
     <row r="3" spans="1:6" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="12">
-        <f>SUM('E-BOM'!M:M)</f>
+        <f>SUM('E-BOM'!N:N)</f>
         <v>35.464000000000006</v>
       </c>
       <c r="E3" s="15"/>
@@ -2702,7 +2699,7 @@
     </row>
     <row r="4" spans="1:6" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="12">
@@ -2715,11 +2712,11 @@
     </row>
     <row r="5" spans="1:6" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="12">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15">
@@ -2728,7 +2725,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="20">
@@ -2742,7 +2739,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C7" s="20">
         <v>3.5</v>
@@ -2755,7 +2752,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C8" s="20">
         <f>SUM(D9:D10)</f>
@@ -2770,7 +2767,7 @@
     </row>
     <row r="9" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B9" s="11" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="13">
@@ -2783,7 +2780,7 @@
     </row>
     <row r="10" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="13">
@@ -2800,11 +2797,11 @@
     </row>
     <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C12" s="24">
         <f>SUM(C2:C10)</f>
-        <v>62.464000000000006</v>
+        <v>64.463999999999999</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16">
@@ -2821,11 +2818,11 @@
     </row>
     <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C14" s="26">
         <f>C12*1000</f>
-        <v>62464.000000000007</v>
+        <v>64464</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="19">
@@ -2845,12 +2842,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC53"/>
+  <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2863,40 +2860,37 @@
     <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.140625" customWidth="1"/>
-    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
@@ -2905,1657 +2899,1636 @@
         <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="I1" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5">
+        <v>10.15</v>
+      </c>
+      <c r="N2" s="5">
+        <f t="shared" ref="N2:N33" si="0">K2*J2</f>
+        <v>10.15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>205</v>
+      </c>
+      <c r="R2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="5">
+        <v>6</v>
+      </c>
+      <c r="N3" s="5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="O3">
+        <f>L3*J3</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>205</v>
+      </c>
+      <c r="R3" t="s">
         <v>187</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R1" s="2" t="s">
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="5">
         <v>6</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="N4" s="5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" t="s">
+        <v>149</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="5">
+        <v>3.42</v>
+      </c>
+      <c r="N5" s="5">
+        <f t="shared" si="0"/>
+        <v>3.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" t="s">
+        <v>208</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="5">
+        <v>1.75</v>
+      </c>
+      <c r="N6" s="5">
+        <f t="shared" si="0"/>
+        <v>1.75</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>205</v>
+      </c>
+      <c r="R6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>164</v>
+      </c>
+      <c r="F7" t="s">
+        <v>140</v>
+      </c>
+      <c r="H7" t="s">
+        <v>185</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1.52</v>
+      </c>
+      <c r="N7" s="5">
+        <f t="shared" si="0"/>
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
         <v>294</v>
       </c>
-      <c r="C2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="5">
+        <v>1.23</v>
+      </c>
+      <c r="N8" s="5">
+        <f t="shared" si="0"/>
+        <v>1.23</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>205</v>
+      </c>
+      <c r="R8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>208</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0.99</v>
+      </c>
+      <c r="N9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.99</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>205</v>
+      </c>
+      <c r="R9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>295</v>
+      </c>
+      <c r="D10" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>147</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0.78</v>
+      </c>
+      <c r="N10" s="5">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>205</v>
+      </c>
+      <c r="R10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>296</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E11" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" t="s">
+        <v>101</v>
+      </c>
+      <c r="H11" t="s">
+        <v>185</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="N11" s="5">
+        <f t="shared" si="0"/>
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>205</v>
+      </c>
+      <c r="R11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>297</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" t="s">
+        <v>179</v>
+      </c>
+      <c r="E12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0.61</v>
+      </c>
+      <c r="N12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.61</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>205</v>
+      </c>
+      <c r="R12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" t="s">
+        <v>175</v>
+      </c>
+      <c r="E13" t="s">
+        <v>176</v>
+      </c>
+      <c r="F13" t="s">
+        <v>146</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="N13" s="5">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>205</v>
+      </c>
+      <c r="R13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>165</v>
+      </c>
+      <c r="E14" t="s">
+        <v>166</v>
+      </c>
+      <c r="F14" t="s">
+        <v>141</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0.42</v>
+      </c>
+      <c r="N14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.42</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>205</v>
+      </c>
+      <c r="R14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>298</v>
+      </c>
+      <c r="C15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" t="s">
         <v>161</v>
       </c>
-      <c r="E2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2">
+      <c r="E15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15">
         <v>1</v>
       </c>
-      <c r="J2" s="5">
-        <v>10.15</v>
-      </c>
-      <c r="M2" s="5">
-        <f t="shared" ref="M2:M33" si="0">J2*I2</f>
-        <v>10.15</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>209</v>
-      </c>
-      <c r="R2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>295</v>
-      </c>
-      <c r="C3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E3" t="s">
-        <v>102</v>
-      </c>
-      <c r="F3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G3" t="s">
-        <v>99</v>
-      </c>
-      <c r="H3" t="s">
-        <v>94</v>
-      </c>
-      <c r="I3">
+      <c r="K15" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="N15" s="5">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>205</v>
+      </c>
+      <c r="R15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>169</v>
+      </c>
+      <c r="E16" t="s">
+        <v>170</v>
+      </c>
+      <c r="F16" t="s">
+        <v>144</v>
+      </c>
+      <c r="H16" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16">
         <v>1</v>
       </c>
-      <c r="J3" s="5">
-        <v>6</v>
-      </c>
-      <c r="M3" s="5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="N3">
-        <f>K3*I3</f>
-        <v>0</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>209</v>
-      </c>
-      <c r="R3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E4" t="s">
-        <v>186</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="5">
-        <v>6</v>
-      </c>
-      <c r="M4" s="5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="s">
-        <v>296</v>
-      </c>
-      <c r="C5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F5" t="s">
-        <v>153</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5" s="5">
-        <v>3.42</v>
-      </c>
-      <c r="M5" s="5">
-        <f t="shared" si="0"/>
-        <v>3.42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E6" t="s">
-        <v>167</v>
-      </c>
-      <c r="F6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H6" t="s">
-        <v>212</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6" s="5">
-        <v>1.75</v>
-      </c>
-      <c r="M6" s="5">
-        <f t="shared" si="0"/>
-        <v>1.75</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>209</v>
-      </c>
-      <c r="R6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" t="s">
-        <v>297</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>168</v>
-      </c>
-      <c r="F7" t="s">
-        <v>144</v>
-      </c>
-      <c r="H7" t="s">
-        <v>189</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7" s="5">
-        <v>1.52</v>
-      </c>
-      <c r="M7" s="5">
-        <f t="shared" si="0"/>
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" t="s">
-        <v>298</v>
-      </c>
-      <c r="D8" t="s">
-        <v>184</v>
-      </c>
-      <c r="E8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8" s="5">
-        <v>1.23</v>
-      </c>
-      <c r="M8" s="5">
-        <f t="shared" si="0"/>
-        <v>1.23</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>209</v>
-      </c>
-      <c r="R8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>106</v>
-      </c>
-      <c r="D9" t="s">
-        <v>163</v>
-      </c>
-      <c r="E9" t="s">
-        <v>164</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" t="s">
-        <v>212</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0.99</v>
-      </c>
-      <c r="M9" s="5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>209</v>
-      </c>
-      <c r="R9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" t="s">
-        <v>299</v>
-      </c>
-      <c r="D10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" t="s">
-        <v>151</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10" s="5">
-        <v>0.78</v>
-      </c>
-      <c r="M10" s="5">
-        <f t="shared" si="0"/>
-        <v>0.78</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>209</v>
-      </c>
-      <c r="R10" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>300</v>
-      </c>
-      <c r="C11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" t="s">
-        <v>162</v>
-      </c>
-      <c r="E11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H11" t="s">
-        <v>189</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0.67700000000000005</v>
-      </c>
-      <c r="M11" s="5">
-        <f t="shared" si="0"/>
-        <v>0.67700000000000005</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>209</v>
-      </c>
-      <c r="R11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>301</v>
-      </c>
-      <c r="C12" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" t="s">
-        <v>183</v>
-      </c>
-      <c r="E12" t="s">
-        <v>113</v>
-      </c>
-      <c r="F12" t="s">
-        <v>113</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12" s="5">
-        <v>0.61</v>
-      </c>
-      <c r="M12" s="5">
-        <f t="shared" si="0"/>
-        <v>0.61</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>209</v>
-      </c>
-      <c r="R12" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>112</v>
-      </c>
-      <c r="D13" t="s">
-        <v>179</v>
-      </c>
-      <c r="E13" t="s">
-        <v>180</v>
-      </c>
-      <c r="F13" t="s">
-        <v>150</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="M13" s="5">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>209</v>
-      </c>
-      <c r="R13" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" t="s">
-        <v>169</v>
-      </c>
-      <c r="E14" t="s">
-        <v>170</v>
-      </c>
-      <c r="F14" t="s">
-        <v>145</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14" s="5">
-        <v>0.42</v>
-      </c>
-      <c r="M14" s="5">
-        <f t="shared" si="0"/>
-        <v>0.42</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>209</v>
-      </c>
-      <c r="R14" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>302</v>
-      </c>
-      <c r="C15" t="s">
-        <v>107</v>
-      </c>
-      <c r="D15" t="s">
-        <v>165</v>
-      </c>
-      <c r="E15" t="s">
-        <v>166</v>
-      </c>
-      <c r="F15" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" t="s">
-        <v>96</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15" s="5">
+      <c r="K16" s="5">
         <v>0.25</v>
       </c>
-      <c r="M15" s="5">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>209</v>
-      </c>
-      <c r="R15" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" t="s">
-        <v>173</v>
-      </c>
-      <c r="E16" t="s">
-        <v>174</v>
-      </c>
-      <c r="F16" t="s">
-        <v>148</v>
-      </c>
-      <c r="H16" t="s">
-        <v>96</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="M16" s="5">
+      <c r="N16" s="5">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F17" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H17" t="s">
-        <v>93</v>
-      </c>
-      <c r="I17">
+        <v>89</v>
+      </c>
+      <c r="J17">
         <v>2</v>
       </c>
-      <c r="J17" s="5">
+      <c r="K17" s="5">
         <v>0.10299999999999999</v>
       </c>
-      <c r="M17" s="5">
+      <c r="N17" s="5">
         <f t="shared" si="0"/>
         <v>0.20599999999999999</v>
       </c>
       <c r="Q17" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="R17" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F18" t="s">
-        <v>147</v>
-      </c>
-      <c r="I18">
+        <v>143</v>
+      </c>
+      <c r="J18">
         <v>1</v>
       </c>
-      <c r="J18" s="5">
+      <c r="K18" s="5">
         <v>0.20200000000000001</v>
       </c>
-      <c r="M18" s="5">
+      <c r="N18" s="5">
         <f t="shared" si="0"/>
         <v>0.20200000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E19" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F19" t="s">
-        <v>152</v>
-      </c>
-      <c r="I19">
+        <v>148</v>
+      </c>
+      <c r="J19">
         <v>1</v>
       </c>
-      <c r="J19" s="5">
+      <c r="K19" s="5">
         <v>0.187</v>
       </c>
-      <c r="M19" s="5">
+      <c r="N19" s="5">
         <f t="shared" si="0"/>
         <v>0.187</v>
       </c>
       <c r="Q19" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="R19" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F20" t="s">
-        <v>146</v>
-      </c>
-      <c r="I20">
+        <v>142</v>
+      </c>
+      <c r="J20">
         <v>1</v>
       </c>
-      <c r="J20" s="5">
+      <c r="K20" s="5">
         <v>0.185</v>
       </c>
-      <c r="M20" s="5">
+      <c r="N20" s="5">
         <f t="shared" si="0"/>
         <v>0.185</v>
       </c>
       <c r="Q20" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="R20" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F21">
         <v>805</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>4</v>
       </c>
-      <c r="J21" s="5">
+      <c r="K21" s="5">
         <v>0.02</v>
       </c>
-      <c r="M21" s="5">
+      <c r="N21" s="5">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
       <c r="Q21" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="R21" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D22" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E22" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F22" t="s">
-        <v>149</v>
-      </c>
-      <c r="I22">
+        <v>145</v>
+      </c>
+      <c r="J22">
         <v>1</v>
       </c>
-      <c r="J22" s="5">
+      <c r="K22" s="5">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="M22" s="5">
+      <c r="N22" s="5">
         <f t="shared" si="0"/>
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E23" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F23" t="s">
-        <v>44</v>
-      </c>
-      <c r="I23">
+        <v>40</v>
+      </c>
+      <c r="J23">
         <v>1</v>
       </c>
-      <c r="J23" s="5">
+      <c r="K23" s="5">
         <v>1.4E-2</v>
       </c>
-      <c r="M23" s="5">
+      <c r="N23" s="5">
         <f t="shared" si="0"/>
         <v>1.4E-2</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F24" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G24" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H24" t="s">
-        <v>93</v>
-      </c>
-      <c r="I24">
+        <v>89</v>
+      </c>
+      <c r="J24">
         <v>5</v>
       </c>
-      <c r="M24" s="5">
+      <c r="N24" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q24" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="R24" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F25" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G25" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H25" t="s">
-        <v>93</v>
-      </c>
-      <c r="I25">
+        <v>89</v>
+      </c>
+      <c r="J25">
         <v>17</v>
       </c>
-      <c r="M25" s="5">
+      <c r="N25" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q25" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="R25" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F26" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G26" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H26" t="s">
-        <v>93</v>
-      </c>
-      <c r="I26">
+        <v>89</v>
+      </c>
+      <c r="J26">
         <v>10</v>
       </c>
-      <c r="M26" s="5">
+      <c r="N26" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q26" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="R26" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F27" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G27" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H27" t="s">
-        <v>93</v>
-      </c>
-      <c r="I27">
+        <v>89</v>
+      </c>
+      <c r="J27">
         <v>2</v>
       </c>
-      <c r="M27" s="5">
+      <c r="N27" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F28" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G28" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H28" t="s">
-        <v>93</v>
-      </c>
-      <c r="I28">
+        <v>89</v>
+      </c>
+      <c r="J28">
         <v>8</v>
       </c>
-      <c r="M28" s="5">
+      <c r="N28" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F29" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G29" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H29" t="s">
-        <v>93</v>
-      </c>
-      <c r="I29">
+        <v>89</v>
+      </c>
+      <c r="J29">
         <v>3</v>
       </c>
-      <c r="M29" s="5">
+      <c r="N29" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F30" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G30" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H30" t="s">
-        <v>93</v>
-      </c>
-      <c r="I30">
+        <v>89</v>
+      </c>
+      <c r="J30">
         <v>2</v>
       </c>
-      <c r="M30" s="5">
+      <c r="N30" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F31" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G31" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H31" t="s">
-        <v>93</v>
-      </c>
-      <c r="I31">
+        <v>89</v>
+      </c>
+      <c r="J31">
         <v>2</v>
       </c>
-      <c r="M31" s="5">
+      <c r="N31" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" t="s">
+        <v>152</v>
+      </c>
+      <c r="G32" t="s">
+        <v>95</v>
+      </c>
+      <c r="H32" t="s">
+        <v>89</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="N32" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" t="s">
+        <v>121</v>
+      </c>
+      <c r="F33" t="s">
+        <v>152</v>
+      </c>
+      <c r="G33" t="s">
+        <v>95</v>
+      </c>
+      <c r="H33" t="s">
+        <v>89</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="N33" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34" t="s">
+        <v>152</v>
+      </c>
+      <c r="G34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H34" t="s">
+        <v>89</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="N34" s="5">
+        <f t="shared" ref="N34:N53" si="1">K34*J34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" t="s">
         <v>66</v>
       </c>
-      <c r="B32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="C35" t="s">
+        <v>123</v>
+      </c>
+      <c r="F35" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" t="s">
+        <v>95</v>
+      </c>
+      <c r="H35" t="s">
+        <v>89</v>
+      </c>
+      <c r="J35">
+        <v>4</v>
+      </c>
+      <c r="N35" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" t="s">
         <v>124</v>
       </c>
-      <c r="F32" t="s">
-        <v>156</v>
-      </c>
-      <c r="G32" t="s">
-        <v>99</v>
-      </c>
-      <c r="H32" t="s">
-        <v>93</v>
-      </c>
-      <c r="I32">
+      <c r="F36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G36" t="s">
+        <v>95</v>
+      </c>
+      <c r="H36" t="s">
+        <v>89</v>
+      </c>
+      <c r="J36">
         <v>1</v>
       </c>
-      <c r="M32" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="N36" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" t="s">
         <v>125</v>
       </c>
-      <c r="F33" t="s">
-        <v>156</v>
-      </c>
-      <c r="G33" t="s">
-        <v>99</v>
-      </c>
-      <c r="H33" t="s">
-        <v>93</v>
-      </c>
-      <c r="I33">
+      <c r="F37" t="s">
+        <v>151</v>
+      </c>
+      <c r="G37" t="s">
+        <v>95</v>
+      </c>
+      <c r="H37" t="s">
+        <v>89</v>
+      </c>
+      <c r="J37">
         <v>1</v>
       </c>
-      <c r="M33" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="N37" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" t="s">
         <v>126</v>
       </c>
-      <c r="F34" t="s">
-        <v>156</v>
-      </c>
-      <c r="G34" t="s">
-        <v>99</v>
-      </c>
-      <c r="H34" t="s">
-        <v>93</v>
-      </c>
-      <c r="I34">
+      <c r="F38" t="s">
+        <v>152</v>
+      </c>
+      <c r="G38" t="s">
+        <v>95</v>
+      </c>
+      <c r="H38" t="s">
+        <v>89</v>
+      </c>
+      <c r="J38">
         <v>2</v>
       </c>
-      <c r="M34" s="5">
-        <f t="shared" ref="M34:M53" si="1">J34*I34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="N38" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>70</v>
       </c>
-      <c r="C35" t="s">
+      <c r="B39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" t="s">
         <v>127</v>
       </c>
-      <c r="F35" t="s">
-        <v>70</v>
-      </c>
-      <c r="G35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H35" t="s">
-        <v>93</v>
-      </c>
-      <c r="I35">
-        <v>4</v>
-      </c>
-      <c r="M35" s="5">
+      <c r="F39" t="s">
+        <v>153</v>
+      </c>
+      <c r="G39" t="s">
+        <v>95</v>
+      </c>
+      <c r="H39" t="s">
+        <v>89</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="N39" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" t="s">
+        <v>128</v>
+      </c>
+      <c r="F40" t="s">
+        <v>154</v>
+      </c>
+      <c r="G40" t="s">
+        <v>95</v>
+      </c>
+      <c r="H40" t="s">
+        <v>89</v>
+      </c>
+      <c r="J40">
+        <v>13</v>
+      </c>
+      <c r="N40" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
         <v>71</v>
       </c>
-      <c r="B36" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" t="s">
-        <v>128</v>
-      </c>
-      <c r="F36" t="s">
-        <v>70</v>
-      </c>
-      <c r="G36" t="s">
-        <v>99</v>
-      </c>
-      <c r="H36" t="s">
-        <v>93</v>
-      </c>
-      <c r="I36">
+      <c r="C41" t="s">
+        <v>129</v>
+      </c>
+      <c r="F41" t="s">
+        <v>153</v>
+      </c>
+      <c r="G41" t="s">
+        <v>95</v>
+      </c>
+      <c r="H41" t="s">
+        <v>89</v>
+      </c>
+      <c r="J41">
         <v>1</v>
       </c>
-      <c r="M36" s="5">
+      <c r="N41" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37" t="s">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" t="s">
+        <v>130</v>
+      </c>
+      <c r="F42" t="s">
+        <v>154</v>
+      </c>
+      <c r="G42" t="s">
+        <v>95</v>
+      </c>
+      <c r="H42" t="s">
+        <v>89</v>
+      </c>
+      <c r="J42">
+        <v>5</v>
+      </c>
+      <c r="N42" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" t="s">
+        <v>131</v>
+      </c>
+      <c r="F43" t="s">
+        <v>153</v>
+      </c>
+      <c r="G43" t="s">
+        <v>95</v>
+      </c>
+      <c r="H43" t="s">
+        <v>89</v>
+      </c>
+      <c r="J43">
+        <v>2</v>
+      </c>
+      <c r="N43" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" t="s">
+        <v>132</v>
+      </c>
+      <c r="F44" t="s">
         <v>155</v>
       </c>
-      <c r="G37" t="s">
-        <v>99</v>
-      </c>
-      <c r="H37" t="s">
-        <v>93</v>
-      </c>
-      <c r="I37">
+      <c r="G44" t="s">
+        <v>95</v>
+      </c>
+      <c r="H44" t="s">
+        <v>89</v>
+      </c>
+      <c r="J44">
         <v>1</v>
       </c>
-      <c r="M37" s="5">
+      <c r="N44" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" t="s">
         <v>73</v>
-      </c>
-      <c r="B38" t="s">
-        <v>60</v>
-      </c>
-      <c r="C38" t="s">
-        <v>130</v>
-      </c>
-      <c r="F38" t="s">
-        <v>156</v>
-      </c>
-      <c r="G38" t="s">
-        <v>99</v>
-      </c>
-      <c r="H38" t="s">
-        <v>93</v>
-      </c>
-      <c r="I38">
-        <v>2</v>
-      </c>
-      <c r="M38" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>74</v>
-      </c>
-      <c r="B39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" t="s">
-        <v>131</v>
-      </c>
-      <c r="F39" t="s">
-        <v>157</v>
-      </c>
-      <c r="G39" t="s">
-        <v>99</v>
-      </c>
-      <c r="H39" t="s">
-        <v>93</v>
-      </c>
-      <c r="I39">
-        <v>1</v>
-      </c>
-      <c r="M39" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" t="s">
-        <v>77</v>
-      </c>
-      <c r="C40" t="s">
-        <v>132</v>
-      </c>
-      <c r="F40" t="s">
-        <v>158</v>
-      </c>
-      <c r="G40" t="s">
-        <v>99</v>
-      </c>
-      <c r="H40" t="s">
-        <v>93</v>
-      </c>
-      <c r="I40">
-        <v>13</v>
-      </c>
-      <c r="M40" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" t="s">
-        <v>133</v>
-      </c>
-      <c r="F41" t="s">
-        <v>157</v>
-      </c>
-      <c r="G41" t="s">
-        <v>99</v>
-      </c>
-      <c r="H41" t="s">
-        <v>93</v>
-      </c>
-      <c r="I41">
-        <v>1</v>
-      </c>
-      <c r="M41" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>79</v>
-      </c>
-      <c r="B42" t="s">
-        <v>77</v>
-      </c>
-      <c r="C42" t="s">
-        <v>134</v>
-      </c>
-      <c r="F42" t="s">
-        <v>158</v>
-      </c>
-      <c r="G42" t="s">
-        <v>99</v>
-      </c>
-      <c r="H42" t="s">
-        <v>93</v>
-      </c>
-      <c r="I42">
-        <v>5</v>
-      </c>
-      <c r="M42" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" t="s">
-        <v>135</v>
-      </c>
-      <c r="F43" t="s">
-        <v>157</v>
-      </c>
-      <c r="G43" t="s">
-        <v>99</v>
-      </c>
-      <c r="H43" t="s">
-        <v>93</v>
-      </c>
-      <c r="I43">
-        <v>2</v>
-      </c>
-      <c r="M43" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>81</v>
-      </c>
-      <c r="B44" t="s">
-        <v>82</v>
-      </c>
-      <c r="C44" t="s">
-        <v>136</v>
-      </c>
-      <c r="F44" t="s">
-        <v>159</v>
-      </c>
-      <c r="G44" t="s">
-        <v>99</v>
-      </c>
-      <c r="H44" t="s">
-        <v>93</v>
-      </c>
-      <c r="I44">
-        <v>1</v>
-      </c>
-      <c r="M44" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>83</v>
-      </c>
-      <c r="B45" t="s">
-        <v>77</v>
       </c>
       <c r="C45">
         <v>10</v>
       </c>
       <c r="F45" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G45" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H45" t="s">
-        <v>93</v>
-      </c>
-      <c r="I45">
+        <v>89</v>
+      </c>
+      <c r="J45">
         <v>1</v>
       </c>
-      <c r="M45" s="5">
+      <c r="N45" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C46">
         <v>20</v>
       </c>
       <c r="F46" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G46" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H46" t="s">
-        <v>93</v>
-      </c>
-      <c r="I46">
+        <v>89</v>
+      </c>
+      <c r="J46">
         <v>2</v>
       </c>
-      <c r="M46" s="5">
+      <c r="N46" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B47" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C47" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F47" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G47" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H47" t="s">
-        <v>93</v>
-      </c>
-      <c r="I47">
+        <v>89</v>
+      </c>
+      <c r="J47">
         <v>1</v>
       </c>
-      <c r="M47" s="5">
+      <c r="N47" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B48" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C48" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F48" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G48" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H48" t="s">
-        <v>93</v>
-      </c>
-      <c r="I48">
+        <v>89</v>
+      </c>
+      <c r="J48">
         <v>1</v>
       </c>
-      <c r="M48" s="5">
+      <c r="N48" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C49">
         <v>330</v>
       </c>
       <c r="F49" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G49" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H49" t="s">
-        <v>93</v>
-      </c>
-      <c r="I49">
+        <v>89</v>
+      </c>
+      <c r="J49">
         <v>1</v>
       </c>
-      <c r="M49" s="5">
+      <c r="N49" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C50">
         <v>380</v>
       </c>
       <c r="F50" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G50" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H50" t="s">
-        <v>93</v>
-      </c>
-      <c r="I50">
+        <v>89</v>
+      </c>
+      <c r="J50">
         <v>2</v>
       </c>
-      <c r="M50" s="5">
+      <c r="N50" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" t="s">
+        <v>135</v>
+      </c>
+      <c r="F51" t="s">
+        <v>154</v>
+      </c>
+      <c r="G51" t="s">
+        <v>95</v>
+      </c>
+      <c r="H51" t="s">
         <v>89</v>
       </c>
-      <c r="B51" t="s">
-        <v>77</v>
-      </c>
-      <c r="C51" t="s">
-        <v>139</v>
-      </c>
-      <c r="F51" t="s">
-        <v>158</v>
-      </c>
-      <c r="G51" t="s">
-        <v>99</v>
-      </c>
-      <c r="H51" t="s">
-        <v>93</v>
-      </c>
-      <c r="I51">
+      <c r="J51">
         <v>2</v>
       </c>
-      <c r="M51" s="5">
+      <c r="N51" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C52" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F52" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G52" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H52" t="s">
-        <v>93</v>
-      </c>
-      <c r="I52">
+        <v>89</v>
+      </c>
+      <c r="J52">
         <v>1</v>
       </c>
-      <c r="M52" s="5">
+      <c r="N52" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C53" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F53" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G53" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H53" t="s">
-        <v>93</v>
-      </c>
-      <c r="I53">
+        <v>89</v>
+      </c>
+      <c r="J53">
         <v>4</v>
       </c>
-      <c r="M53" s="5">
+      <c r="N53" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:AC53">
-    <sortCondition descending="1" ref="M1:M53"/>
+  <sortState ref="A1:AE53">
+    <sortCondition descending="1" ref="N1:N53"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>